<commit_message>
feat(smart-health): update DDL and add DML
</commit_message>
<xml_diff>
--- a/content/fintech-accelator/data/Normalizacion-4FN.xlsx
+++ b/content/fintech-accelator/data/Normalizacion-4FN.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\study_2025\Documents\Github\Doc-UP-AlejandroJaimes\sql-101-mastering\content\fintech-accelator\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gisel\OneDrive\Documentos\GitHub\gisell3010\sql-101-mastering\content\fintech-accelator\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE9BEF37-EF0B-4054-BFB2-A2066FD69BF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1F0F5C-0341-481B-97FA-1C28B87073B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6105" yWindow="1080" windowWidth="28800" windowHeight="15810" xr2:uid="{8032EE73-E59F-429D-B5B7-DB3D5A480306}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{8032EE73-E59F-429D-B5B7-DB3D5A480306}"/>
   </bookViews>
   <sheets>
     <sheet name="Coceptualizacion" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1410,6 +1413,12 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1419,9 +1428,60 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1433,63 +1493,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2121,52 +2124,52 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B98D47-5E39-452C-A9E6-D9709EFE7CF6}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.28515625" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.42578125" customWidth="1"/>
-    <col min="5" max="5" width="3.85546875" customWidth="1"/>
-    <col min="6" max="6" width="6.140625" customWidth="1"/>
-    <col min="7" max="8" width="11.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1"/>
+    <col min="3" max="3" width="15.44140625" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="5" max="5" width="3.88671875" customWidth="1"/>
+    <col min="6" max="6" width="6.109375" customWidth="1"/>
+    <col min="7" max="8" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+    <row r="2" spans="1:9" ht="97.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="40" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="40"/>
-      <c r="C4" s="40"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2176,13 +2179,13 @@
       <c r="C5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E5" s="44"/>
+      <c r="F5" s="44"/>
+      <c r="G5" s="44"/>
+      <c r="H5" s="44"/>
+      <c r="I5" s="44"/>
+    </row>
+    <row r="6" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>2</v>
       </c>
@@ -2192,13 +2195,13 @@
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-    </row>
-    <row r="7" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+    </row>
+    <row r="7" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
@@ -2208,13 +2211,13 @@
       <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-    </row>
-    <row r="8" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+    </row>
+    <row r="8" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>4</v>
       </c>
@@ -2224,13 +2227,13 @@
       <c r="C8" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-    </row>
-    <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+    </row>
+    <row r="9" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="15" t="s">
         <v>5</v>
       </c>
@@ -2261,51 +2264,51 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" customWidth="1"/>
-    <col min="10" max="10" width="31.5703125" customWidth="1"/>
-    <col min="11" max="11" width="22.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" customWidth="1"/>
-    <col min="14" max="14" width="21.5703125" customWidth="1"/>
-    <col min="16" max="16" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
+    <col min="9" max="9" width="22.88671875" customWidth="1"/>
+    <col min="10" max="10" width="31.5546875" customWidth="1"/>
+    <col min="11" max="11" width="22.88671875" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" customWidth="1"/>
+    <col min="14" max="14" width="21.5546875" customWidth="1"/>
+    <col min="16" max="16" width="14.33203125" customWidth="1"/>
     <col min="17" max="17" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:10" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="G3" s="47" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="G3" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>18</v>
       </c>
@@ -2316,7 +2319,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>165</v>
       </c>
@@ -2327,21 +2330,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
         <v>166</v>
       </c>
@@ -2351,7 +2354,7 @@
       <c r="E9" s="48"/>
       <c r="F9" s="48"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>167</v>
       </c>
@@ -2371,17 +2374,17 @@
         <v>172</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="74.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="28" t="s">
         <v>173</v>
       </c>
       <c r="B11" s="29" t="s">
         <v>174</v>
       </c>
-      <c r="C11" s="65">
+      <c r="C11" s="40">
         <v>36891</v>
       </c>
-      <c r="D11" s="66" t="s">
+      <c r="D11" s="41" t="s">
         <v>175</v>
       </c>
       <c r="E11" s="28">
@@ -2391,30 +2394,30 @@
         <v>176</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="43"/>
-      <c r="B12" s="43"/>
-      <c r="C12" s="43"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="59"/>
+      <c r="B12" s="59"/>
+      <c r="C12" s="59"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="48" t="s">
         <v>79</v>
       </c>
@@ -2424,7 +2427,7 @@
       <c r="E17" s="48"/>
       <c r="F17" s="48"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="26" t="s">
         <v>71</v>
       </c>
@@ -2444,7 +2447,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A19" s="29">
         <v>1</v>
       </c>
@@ -2464,7 +2467,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="20">
         <v>1</v>
       </c>
@@ -2484,7 +2487,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="20">
         <v>1</v>
       </c>
@@ -2500,34 +2503,34 @@
       <c r="E21" s="20"/>
       <c r="F21" s="20"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="58" t="s">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="59"/>
-      <c r="C24" s="59"/>
-      <c r="D24" s="59"/>
-      <c r="E24" s="60"/>
-    </row>
-    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="53" t="s">
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
+      <c r="D24" s="61"/>
+      <c r="E24" s="62"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B25" s="53"/>
-      <c r="C25" s="53"/>
-      <c r="D25" s="53"/>
-      <c r="E25" s="53"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A27" s="48" t="s">
         <v>79</v>
       </c>
       <c r="B27" s="48"/>
       <c r="C27" s="48"/>
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="64"/>
+      <c r="F27" s="46"/>
       <c r="H27" s="48" t="s">
         <v>94</v>
       </c>
@@ -2535,7 +2538,7 @@
       <c r="J27" s="48"/>
       <c r="K27" s="48"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A28" s="20" t="s">
         <v>71</v>
       </c>
@@ -2564,7 +2567,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20">
         <v>1</v>
       </c>
@@ -2593,7 +2596,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E30" s="20">
         <v>2</v>
       </c>
@@ -2613,7 +2616,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="E31" s="20">
         <v>3</v>
       </c>
@@ -2633,56 +2636,56 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A36" s="54" t="s">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A36" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B36" s="55"/>
-      <c r="C36" s="55"/>
-      <c r="D36" s="55"/>
-      <c r="E36" s="56"/>
-    </row>
-    <row r="37" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="53" t="s">
+      <c r="B36" s="56"/>
+      <c r="C36" s="56"/>
+      <c r="D36" s="56"/>
+      <c r="E36" s="57"/>
+    </row>
+    <row r="37" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="B37" s="53"/>
-      <c r="C37" s="53"/>
-      <c r="D37" s="53"/>
-      <c r="E37" s="53"/>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B37" s="54"/>
+      <c r="C37" s="54"/>
+      <c r="D37" s="54"/>
+      <c r="E37" s="54"/>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39" s="48" t="s">
         <v>79</v>
       </c>
       <c r="B39" s="48"/>
       <c r="C39" s="48"/>
-      <c r="E39" s="62" t="s">
+      <c r="E39" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="F39" s="64"/>
-      <c r="H39" s="62" t="s">
+      <c r="F39" s="46"/>
+      <c r="H39" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="I39" s="63"/>
-      <c r="J39" s="64"/>
-      <c r="M39" s="62" t="s">
+      <c r="I39" s="47"/>
+      <c r="J39" s="46"/>
+      <c r="M39" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="N39" s="64"/>
-      <c r="P39" s="62" t="s">
+      <c r="N39" s="46"/>
+      <c r="P39" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="Q39" s="64"/>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="Q39" s="46"/>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40" s="20" t="s">
         <v>71</v>
       </c>
@@ -2720,7 +2723,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="41" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="20">
         <v>1</v>
       </c>
@@ -2758,7 +2761,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="42" spans="1:17" ht="30" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
       <c r="E42" s="20">
         <v>2</v>
       </c>
@@ -2787,7 +2790,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="E43" s="20">
         <v>3</v>
       </c>
@@ -2804,37 +2807,37 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A48" s="49" t="s">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A48" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B48" s="50"/>
-      <c r="C48" s="50"/>
-      <c r="D48" s="50"/>
-      <c r="E48" s="51"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A49" s="52" t="s">
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="51"/>
+      <c r="E48" s="52"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A49" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="53"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="53"/>
-      <c r="E49" s="53"/>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" s="61" t="s">
+      <c r="B49" s="54"/>
+      <c r="C49" s="54"/>
+      <c r="D49" s="54"/>
+      <c r="E49" s="54"/>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A51" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="B51" s="61"/>
-      <c r="C51" s="61"/>
-      <c r="I51" s="62" t="s">
+      <c r="B51" s="49"/>
+      <c r="C51" s="49"/>
+      <c r="I51" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="J51" s="63"/>
-      <c r="K51" s="64"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J51" s="47"/>
+      <c r="K51" s="46"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A52" s="20" t="s">
         <v>71</v>
       </c>
@@ -2854,7 +2857,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A53" s="20">
         <v>1</v>
       </c>
@@ -2874,7 +2877,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I54" s="20">
         <v>2</v>
       </c>
@@ -2885,7 +2888,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I55" s="20">
         <v>3</v>
       </c>
@@ -2896,7 +2899,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
         <v>99</v>
       </c>
@@ -2908,7 +2911,7 @@
       <c r="F56" s="48"/>
       <c r="G56" s="48"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A57" s="26" t="s">
         <v>71</v>
       </c>
@@ -2927,12 +2930,12 @@
       <c r="G57" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="I57" s="62" t="s">
+      <c r="I57" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="J57" s="64"/>
-    </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J57" s="46"/>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A58" s="20">
         <v>1</v>
       </c>
@@ -2958,7 +2961,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A59" s="20">
         <v>2</v>
       </c>
@@ -2984,7 +2987,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I60" s="20">
         <v>2</v>
       </c>
@@ -2992,7 +2995,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.3">
       <c r="I61" s="20">
         <v>3</v>
       </c>
@@ -3000,17 +3003,17 @@
         <v>87</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" s="62" t="s">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A62" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="B62" s="64"/>
-      <c r="E62" s="62" t="s">
+      <c r="B62" s="46"/>
+      <c r="E62" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="F62" s="64"/>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="F62" s="46"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A63" s="26" t="s">
         <v>71</v>
       </c>
@@ -3024,7 +3027,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="20">
         <v>1</v>
       </c>
@@ -3038,7 +3041,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A65" s="20">
         <v>2</v>
       </c>
@@ -3054,20 +3057,13 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="P39:Q39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="H27:K27"/>
-    <mergeCell ref="M39:N39"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="A51:C51"/>
-    <mergeCell ref="I51:K51"/>
-    <mergeCell ref="I57:J57"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A9:F9"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A49:E49"/>
     <mergeCell ref="A36:E36"/>
@@ -3078,13 +3074,20 @@
     <mergeCell ref="A25:E25"/>
     <mergeCell ref="A17:F17"/>
     <mergeCell ref="A39:C39"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A51:C51"/>
+    <mergeCell ref="I51:K51"/>
+    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="E56:G56"/>
+    <mergeCell ref="P39:Q39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="H27:K27"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="E39:F39"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="D11" r:id="rId1" xr:uid="{B93D31B2-8990-43D3-9623-D57A887E828F}"/>
@@ -3115,16 +3118,16 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>160</v>
       </c>
       <c r="B1" s="48"/>
       <c r="C1" s="48"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="26" t="s">
         <v>161</v>
       </c>
@@ -3135,17 +3138,17 @@
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="43" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="59" t="s">
         <v>160</v>
       </c>
-      <c r="B4" s="43"/>
-      <c r="E4" s="43" t="s">
+      <c r="B4" s="59"/>
+      <c r="E4" s="59" t="s">
         <v>163</v>
       </c>
-      <c r="F4" s="43"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -3173,57 +3176,57 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BA7B19D-F6C6-4765-A152-E78D9B15BA8A}">
   <dimension ref="A1:U62"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="M48" sqref="M48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.109375" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
-    <col min="9" max="10" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.5546875" customWidth="1"/>
+    <col min="9" max="10" width="17.88671875" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="G3" s="47" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="G3" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>18</v>
       </c>
@@ -3234,7 +3237,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>104</v>
       </c>
@@ -3245,21 +3248,21 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="48" t="s">
         <v>104</v>
       </c>
@@ -3274,7 +3277,7 @@
       <c r="J9" s="48"/>
       <c r="K9" s="48"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="33" t="s">
         <v>105</v>
       </c>
@@ -3309,7 +3312,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
         <v>106</v>
       </c>
@@ -3344,7 +3347,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
         <v>124</v>
       </c>
@@ -3379,43 +3382,43 @@
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="57" t="s">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="57"/>
-      <c r="C14" s="57"/>
-      <c r="D14" s="57"/>
-      <c r="E14" s="57"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="43" t="s">
+      <c r="B14" s="58"/>
+      <c r="C14" s="58"/>
+      <c r="D14" s="58"/>
+      <c r="E14" s="58"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A19" s="58" t="s">
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A19" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="59"/>
-      <c r="E19" s="60"/>
-    </row>
-    <row r="20" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="61"/>
+      <c r="E19" s="62"/>
+    </row>
+    <row r="20" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B20" s="53"/>
-      <c r="C20" s="53"/>
-      <c r="D20" s="53"/>
-      <c r="E20" s="53"/>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="54"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="54"/>
+      <c r="E20" s="54"/>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="48" t="s">
         <v>135</v>
       </c>
@@ -3440,7 +3443,7 @@
       <c r="T22" s="48"/>
       <c r="U22" s="48"/>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" s="34" t="s">
         <v>105</v>
       </c>
@@ -3487,7 +3490,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" s="29" t="s">
         <v>106</v>
       </c>
@@ -3534,7 +3537,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" s="29" t="s">
         <v>124</v>
       </c>
@@ -3581,7 +3584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F26" s="23">
         <v>3</v>
       </c>
@@ -3589,32 +3592,32 @@
         <v>136</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A31" s="54" t="s">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A31" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="55"/>
-      <c r="C31" s="55"/>
-      <c r="D31" s="55"/>
-      <c r="E31" s="56"/>
-    </row>
-    <row r="32" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53" t="s">
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="57"/>
+    </row>
+    <row r="32" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="B32" s="53"/>
-      <c r="C32" s="53"/>
-      <c r="D32" s="53"/>
-      <c r="E32" s="53"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="54"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="54"/>
+      <c r="E32" s="54"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" s="48" t="s">
         <v>135</v>
       </c>
@@ -3625,15 +3628,15 @@
         <v>137</v>
       </c>
       <c r="G34" s="48"/>
-      <c r="I34" s="62" t="s">
+      <c r="I34" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="J34" s="64"/>
-      <c r="L34" s="62" t="s">
+      <c r="J34" s="46"/>
+      <c r="L34" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="M34" s="63"/>
-      <c r="N34" s="64"/>
+      <c r="M34" s="47"/>
+      <c r="N34" s="46"/>
       <c r="P34" s="48" t="s">
         <v>141</v>
       </c>
@@ -3643,7 +3646,7 @@
       <c r="T34" s="48"/>
       <c r="U34" s="48"/>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="34" t="s">
         <v>105</v>
       </c>
@@ -3696,7 +3699,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="29" t="s">
         <v>106</v>
       </c>
@@ -3749,7 +3752,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="29" t="s">
         <v>124</v>
       </c>
@@ -3802,7 +3805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F38" s="23">
         <v>3</v>
       </c>
@@ -3810,25 +3813,25 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A43" s="49" t="s">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A43" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="51"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A44" s="52" t="s">
+      <c r="B43" s="51"/>
+      <c r="C43" s="51"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="52"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A44" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B44" s="53"/>
-      <c r="C44" s="53"/>
-      <c r="D44" s="53"/>
-      <c r="E44" s="53"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B44" s="54"/>
+      <c r="C44" s="54"/>
+      <c r="D44" s="54"/>
+      <c r="E44" s="54"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="48" t="s">
         <v>135</v>
       </c>
@@ -3839,15 +3842,15 @@
         <v>137</v>
       </c>
       <c r="G46" s="48"/>
-      <c r="I46" s="62" t="s">
+      <c r="I46" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="J46" s="64"/>
-      <c r="L46" s="62" t="s">
+      <c r="J46" s="46"/>
+      <c r="L46" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="M46" s="63"/>
-      <c r="N46" s="64"/>
+      <c r="M46" s="47"/>
+      <c r="N46" s="46"/>
       <c r="P46" s="48" t="s">
         <v>141</v>
       </c>
@@ -3857,7 +3860,7 @@
       <c r="T46" s="48"/>
       <c r="U46" s="48"/>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="34" t="s">
         <v>105</v>
       </c>
@@ -3910,7 +3913,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="29" t="s">
         <v>106</v>
       </c>
@@ -3963,7 +3966,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="29" t="s">
         <v>124</v>
       </c>
@@ -4016,7 +4019,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="F50" s="23">
         <v>3</v>
       </c>
@@ -4024,17 +4027,17 @@
         <v>136</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P53" s="62" t="s">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P53" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="Q53" s="64"/>
-      <c r="S53" s="62" t="s">
+      <c r="Q53" s="46"/>
+      <c r="S53" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="T53" s="64"/>
-    </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T53" s="46"/>
+    </row>
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P54" s="25" t="s">
         <v>71</v>
       </c>
@@ -4048,7 +4051,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P55" s="23">
         <v>1</v>
       </c>
@@ -4062,7 +4065,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P56" s="23">
         <v>2</v>
       </c>
@@ -4076,17 +4079,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="P59" s="62" t="s">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="P59" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="Q59" s="64"/>
-      <c r="S59" s="62" t="s">
+      <c r="Q59" s="46"/>
+      <c r="S59" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="T59" s="64"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="T59" s="46"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P60" s="25" t="s">
         <v>71</v>
       </c>
@@ -4100,7 +4103,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P61" s="23">
         <v>1</v>
       </c>
@@ -4114,7 +4117,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P62" s="23">
         <v>2</v>
       </c>
@@ -4130,12 +4133,21 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="P53:Q53"/>
-    <mergeCell ref="S53:T53"/>
-    <mergeCell ref="P59:Q59"/>
-    <mergeCell ref="S59:T59"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="P34:U34"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:K9"/>
+    <mergeCell ref="A22:D22"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="A31:E31"/>
+    <mergeCell ref="A32:E32"/>
+    <mergeCell ref="I22:K22"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A15:E15"/>
+    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A20:E20"/>
     <mergeCell ref="P22:U22"/>
     <mergeCell ref="A34:D34"/>
     <mergeCell ref="F34:G34"/>
@@ -4145,23 +4157,14 @@
     <mergeCell ref="I46:J46"/>
     <mergeCell ref="L46:N46"/>
     <mergeCell ref="P46:U46"/>
-    <mergeCell ref="A9:K9"/>
-    <mergeCell ref="A22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="A31:E31"/>
-    <mergeCell ref="A32:E32"/>
-    <mergeCell ref="I22:K22"/>
     <mergeCell ref="A43:E43"/>
     <mergeCell ref="A44:E44"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A15:E15"/>
-    <mergeCell ref="A19:E19"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="P53:Q53"/>
+    <mergeCell ref="S53:T53"/>
+    <mergeCell ref="P59:Q59"/>
+    <mergeCell ref="S59:T59"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="P34:U34"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4189,56 +4192,56 @@
       <selection activeCell="F42" sqref="F42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="44.140625" customWidth="1"/>
-    <col min="4" max="4" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.7109375" customWidth="1"/>
-    <col min="8" max="8" width="18.5703125" customWidth="1"/>
-    <col min="9" max="10" width="17.85546875" customWidth="1"/>
+    <col min="2" max="2" width="31.44140625" customWidth="1"/>
+    <col min="3" max="3" width="44.109375" customWidth="1"/>
+    <col min="4" max="4" width="26.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.88671875" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" customWidth="1"/>
+    <col min="7" max="7" width="23.6640625" customWidth="1"/>
+    <col min="8" max="8" width="18.5546875" customWidth="1"/>
+    <col min="9" max="10" width="17.88671875" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="14" max="14" width="17.7109375" customWidth="1"/>
-    <col min="15" max="15" width="22.28515625" customWidth="1"/>
-    <col min="17" max="17" width="21.7109375" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" customWidth="1"/>
-    <col min="19" max="19" width="17.85546875" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="22.42578125" customWidth="1"/>
+    <col min="14" max="14" width="17.6640625" customWidth="1"/>
+    <col min="15" max="15" width="22.33203125" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" customWidth="1"/>
+    <col min="18" max="18" width="15.44140625" customWidth="1"/>
+    <col min="19" max="19" width="17.88671875" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" customWidth="1"/>
+    <col min="21" max="21" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:11" ht="23.4" x14ac:dyDescent="0.45">
+      <c r="A1" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
       <c r="H1" s="17"/>
       <c r="I1" s="17"/>
       <c r="J1" s="17"/>
       <c r="K1" s="17"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="46" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="65" t="s">
         <v>77</v>
       </c>
-      <c r="B3" s="46"/>
-      <c r="C3" s="46"/>
-      <c r="G3" s="47" t="s">
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="G3" s="66" t="s">
         <v>78</v>
       </c>
-      <c r="H3" s="47"/>
-      <c r="I3" s="47"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>18</v>
       </c>
@@ -4249,7 +4252,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="20" t="s">
         <v>146</v>
       </c>
@@ -4260,28 +4263,28 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="44" t="s">
+    <row r="7" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="62" t="s">
+      <c r="B7" s="63"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A8" s="59"/>
+      <c r="B8" s="59"/>
+      <c r="C8" s="59"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="63"/>
-      <c r="C9" s="64"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="47"/>
+      <c r="C9" s="46"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="26" t="s">
         <v>71</v>
       </c>
@@ -4292,7 +4295,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="29">
         <v>1</v>
       </c>
@@ -4303,48 +4306,48 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A13" s="58" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="43" t="s">
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A18" s="58" t="s">
+      <c r="B14" s="59"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="59"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A18" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
-    </row>
-    <row r="19" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="53" t="s">
+      <c r="B18" s="61"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="62"/>
+    </row>
+    <row r="19" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="54" t="s">
         <v>74</v>
       </c>
-      <c r="B19" s="53"/>
-      <c r="C19" s="53"/>
-      <c r="D19" s="53"/>
-      <c r="E19" s="53"/>
-    </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A21" s="62" t="s">
+      <c r="B19" s="54"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A21" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="B21" s="63"/>
-      <c r="C21" s="64"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="46"/>
       <c r="E21" s="48" t="s">
         <v>147</v>
       </c>
@@ -4360,7 +4363,7 @@
       <c r="T21" s="48"/>
       <c r="U21" s="48"/>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="26" t="s">
         <v>71</v>
       </c>
@@ -4401,7 +4404,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="29">
         <v>1</v>
       </c>
@@ -4442,7 +4445,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="P24" s="20">
         <v>2</v>
       </c>
@@ -4462,25 +4465,25 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A30" s="54" t="s">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A30" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="B30" s="55"/>
-      <c r="C30" s="55"/>
-      <c r="D30" s="55"/>
-      <c r="E30" s="56"/>
-    </row>
-    <row r="31" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53" t="s">
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="57"/>
+    </row>
+    <row r="31" spans="1:21" ht="31.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="54" t="s">
         <v>75</v>
       </c>
-      <c r="B31" s="53"/>
-      <c r="C31" s="53"/>
-      <c r="D31" s="53"/>
-      <c r="E31" s="53"/>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="B31" s="54"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="54"/>
+      <c r="E31" s="54"/>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="E32" s="48" t="s">
         <v>147</v>
       </c>
@@ -4491,17 +4494,17 @@
       </c>
       <c r="J32" s="48"/>
       <c r="K32" s="48"/>
-      <c r="N32" s="62" t="s">
+      <c r="N32" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="O32" s="64"/>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A33" s="62" t="s">
+      <c r="O32" s="46"/>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A33" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="B33" s="63"/>
-      <c r="C33" s="64"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="46"/>
       <c r="E33" s="26" t="s">
         <v>71</v>
       </c>
@@ -4527,7 +4530,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34" s="26" t="s">
         <v>71</v>
       </c>
@@ -4562,7 +4565,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="29">
         <v>1</v>
       </c>
@@ -4573,7 +4576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37" s="48" t="s">
         <v>146</v>
       </c>
@@ -4585,12 +4588,12 @@
       </c>
       <c r="G37" s="48"/>
       <c r="H37" s="48"/>
-      <c r="K37" s="62" t="s">
+      <c r="K37" s="45" t="s">
         <v>151</v>
       </c>
-      <c r="L37" s="64"/>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L37" s="46"/>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38" s="26" t="s">
         <v>71</v>
       </c>
@@ -4619,7 +4622,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="39" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" s="29">
         <v>1</v>
       </c>
@@ -4648,33 +4651,31 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A42" s="49" t="s">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A42" s="50" t="s">
         <v>5</v>
       </c>
-      <c r="B42" s="50"/>
-      <c r="C42" s="50"/>
-      <c r="D42" s="50"/>
-      <c r="E42" s="51"/>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A43" s="52" t="s">
+      <c r="B42" s="51"/>
+      <c r="C42" s="51"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="52"/>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A43" s="53" t="s">
         <v>76</v>
       </c>
-      <c r="B43" s="53"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="53"/>
+      <c r="B43" s="54"/>
+      <c r="C43" s="54"/>
+      <c r="D43" s="54"/>
+      <c r="E43" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A21:C21"/>
-    <mergeCell ref="E21:H21"/>
-    <mergeCell ref="A13:E13"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A18:E18"/>
-    <mergeCell ref="A19:E19"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="G3:I3"/>
+    <mergeCell ref="A7:E7"/>
+    <mergeCell ref="A8:C8"/>
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A42:E42"/>
     <mergeCell ref="A43:E43"/>
@@ -4687,11 +4688,13 @@
     <mergeCell ref="K37:L37"/>
     <mergeCell ref="I32:K32"/>
     <mergeCell ref="E32:G32"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="G3:I3"/>
-    <mergeCell ref="A7:E7"/>
-    <mergeCell ref="A8:C8"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A21:C21"/>
+    <mergeCell ref="E21:H21"/>
+    <mergeCell ref="A13:E13"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A18:E18"/>
+    <mergeCell ref="A19:E19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -4719,14 +4722,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="18.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
@@ -4737,7 +4740,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -4748,7 +4751,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="18" t="s">
         <v>23</v>
       </c>
@@ -4759,7 +4762,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>23</v>
       </c>
@@ -4770,7 +4773,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="18" t="s">
         <v>23</v>
       </c>
@@ -4781,7 +4784,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="19" t="s">
         <v>23</v>
       </c>
@@ -4790,7 +4793,7 @@
       </c>
       <c r="C6" s="2"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="18" t="s">
         <v>23</v>
       </c>
@@ -4799,7 +4802,7 @@
       </c>
       <c r="C7" s="2"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="19" t="s">
         <v>23</v>
       </c>
@@ -4808,7 +4811,7 @@
       </c>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="18" t="s">
         <v>23</v>
       </c>
@@ -4817,7 +4820,7 @@
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>23</v>
       </c>
@@ -4826,7 +4829,7 @@
       </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="18" t="s">
         <v>23</v>
       </c>
@@ -4835,7 +4838,7 @@
       </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="19" t="s">
         <v>33</v>
       </c>
@@ -4844,7 +4847,7 @@
       </c>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="18" t="s">
         <v>33</v>
       </c>
@@ -4853,7 +4856,7 @@
       </c>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="19" t="s">
         <v>33</v>
       </c>
@@ -4862,7 +4865,7 @@
       </c>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="18" t="s">
         <v>37</v>
       </c>
@@ -4871,7 +4874,7 @@
       </c>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="19" t="s">
         <v>37</v>
       </c>
@@ -4880,7 +4883,7 @@
       </c>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="18" t="s">
         <v>37</v>
       </c>
@@ -4889,7 +4892,7 @@
       </c>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="19" t="s">
         <v>37</v>
       </c>
@@ -4898,7 +4901,7 @@
       </c>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="18" t="s">
         <v>42</v>
       </c>
@@ -4907,7 +4910,7 @@
       </c>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" s="19" t="s">
         <v>44</v>
       </c>
@@ -4916,7 +4919,7 @@
       </c>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="18" t="s">
         <v>46</v>
       </c>
@@ -4925,7 +4928,7 @@
       </c>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="19" t="s">
         <v>47</v>
       </c>
@@ -4934,7 +4937,7 @@
       </c>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" s="18" t="s">
         <v>47</v>
       </c>
@@ -4943,7 +4946,7 @@
       </c>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" s="19" t="s">
         <v>47</v>
       </c>
@@ -4952,7 +4955,7 @@
       </c>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="18" t="s">
         <v>51</v>
       </c>
@@ -4961,7 +4964,7 @@
       </c>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="19" t="s">
         <v>53</v>
       </c>
@@ -4970,7 +4973,7 @@
       </c>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="18" t="s">
         <v>53</v>
       </c>
@@ -4979,7 +4982,7 @@
       </c>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" s="19" t="s">
         <v>56</v>
       </c>
@@ -4988,7 +4991,7 @@
       </c>
       <c r="C28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
         <v>58</v>
       </c>
@@ -4997,7 +5000,7 @@
       </c>
       <c r="C29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" s="19" t="s">
         <v>58</v>
       </c>
@@ -5006,7 +5009,7 @@
       </c>
       <c r="C30" s="2"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" s="18" t="s">
         <v>58</v>
       </c>
@@ -5015,7 +5018,7 @@
       </c>
       <c r="C31" s="2"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" s="19" t="s">
         <v>58</v>
       </c>
@@ -5024,7 +5027,7 @@
       </c>
       <c r="C32" s="2"/>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" s="18" t="s">
         <v>58</v>
       </c>
@@ -5033,123 +5036,123 @@
       </c>
       <c r="C33" s="2"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>

</xml_diff>